<commit_message>
add gr and ud data
</commit_message>
<xml_diff>
--- a/public/data_source/departments.xlsx
+++ b/public/data_source/departments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maldebasi\Desktop\البيانات المفتوحة 1445\البيانات 1445\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\elhawy\projects\seu_public_data\public\data_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{468514B8-9C8B-4665-9202-86F1A730F04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34F52A-06DF-47EC-A127-474FEA5FEC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
   <si>
     <t>code</t>
   </si>
@@ -144,17 +144,110 @@
   </si>
   <si>
     <t>Public Health</t>
+  </si>
+  <si>
+    <t>الحلقوق</t>
+  </si>
+  <si>
+    <t>التجارة الإلكترونية</t>
+  </si>
+  <si>
+    <t>EMED</t>
+  </si>
+  <si>
+    <t>Electronic Media</t>
+  </si>
+  <si>
+    <t>الإعلام الرقمي</t>
+  </si>
+  <si>
+    <t>إدارة مالية</t>
+  </si>
+  <si>
+    <t>اللغة الإنجليزية والترجمة</t>
+  </si>
+  <si>
+    <t>القانون</t>
+  </si>
+  <si>
+    <t>الصحة العامة</t>
+  </si>
+  <si>
+    <t>MCYS</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>الأمن السيبراني</t>
+  </si>
+  <si>
+    <t>DATS</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>علوم البيانات</t>
+  </si>
+  <si>
+    <t>TTEC</t>
+  </si>
+  <si>
+    <t>Translation Technologies</t>
+  </si>
+  <si>
+    <t>تقنيات الترجمة</t>
+  </si>
+  <si>
+    <t>EMBA</t>
+  </si>
+  <si>
+    <t>Executive MBA</t>
+  </si>
+  <si>
+    <t>إدارة الاعمال التنفيذي</t>
+  </si>
+  <si>
+    <t>DMKT</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>التسويق الرقمي</t>
+  </si>
+  <si>
+    <t>DENG</t>
+  </si>
+  <si>
+    <t>English Diploma</t>
+  </si>
+  <si>
+    <t>دبلوم اللغة الإنجليزية</t>
+  </si>
+  <si>
+    <t>HQS</t>
+  </si>
+  <si>
+    <t>Executive Master of Healthcare Quality and Patient Safety</t>
+  </si>
+  <si>
+    <t>الماجستير التنفيذي لجودة الرعاية الصحية و سلامة المرضى</t>
+  </si>
+  <si>
+    <t>الصحه العامه</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -169,6 +262,23 @@
       <sz val="12"/>
       <color rgb="FF002060"/>
       <name val="Frutiger LT Arabic 55 Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,10 +330,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -237,8 +348,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,22 +641,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="A13:D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.125" customWidth="1"/>
-    <col min="2" max="2" width="30.625" customWidth="1"/>
-    <col min="3" max="3" width="25.375" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" customHeight="1">
+    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -555,7 +670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -569,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5">
+    <row r="3" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -583,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5">
+    <row r="4" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -597,7 +712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5">
+    <row r="5" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -611,7 +726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -625,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5">
+    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -639,7 +754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33">
+    <row r="8" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -650,10 +765,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -667,7 +782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25">
+    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -681,7 +796,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -692,10 +807,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -706,7 +821,273 @@
         <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -716,6 +1097,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034A83DF2E6634443A349C17868A69B47" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75be40817d16b9a669dd65bc569c5e8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="39fd7eea-bd78-4e0b-bb05-937733995018" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f855aa50b178639402115d648588c2e" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -872,15 +1262,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -891,13 +1272,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15C50796-8F01-4863-955D-6302365E5BDC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1FAF45-6BBF-47B7-8C4A-CABAD5275E2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1FAF45-6BBF-47B7-8C4A-CABAD5275E2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15C50796-8F01-4863-955D-6302365E5BDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="39fd7eea-bd78-4e0b-bb05-937733995018"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CB9857-AD24-4A7A-99AC-740EBAF5D222}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CB9857-AD24-4A7A-99AC-740EBAF5D222}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>